<commit_message>
Added Apache PO for Excel Reading, and SearchTest Case
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/test-data.xlsx
+++ b/src/test/resources/excels/test-data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ableToSearchProducts" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -17,6 +17,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Product Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product  Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canon EOS 5D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$98.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Galaxy Tab 10.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$241.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacBook Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$1,202.00</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,7 +140,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -120,7 +150,40 @@
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added Reporting. (ReportNG - which is decommissioned)
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/test-data.xlsx
+++ b/src/test/resources/excels/test-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">$1,202.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$0</t>
   </si>
 </sst>
 </file>
@@ -140,10 +146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,6 +189,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added a new case - AddToCart, and added common actions.
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/test-data.xlsx
+++ b/src/test/resources/excels/test-data.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ableToSearchProducts" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ableToAddToCart" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t xml:space="preserve">Product Name</t>
   </si>
@@ -50,6 +51,18 @@
   </si>
   <si>
     <t xml:space="preserve">$0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikon D300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPod Shuffle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$122.00</t>
   </si>
 </sst>
 </file>
@@ -148,8 +161,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -206,4 +219,75 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Made DataProvider to N Elements.
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/test-data.xlsx
+++ b/src/test/resources/excels/test-data.xlsx
@@ -23,10 +23,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
-    <t xml:space="preserve">Product Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product  Price</t>
+    <t xml:space="preserve">ProductName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProductPrice</t>
   </si>
   <si>
     <t xml:space="preserve">Canon EOS 5D</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">$0</t>
   </si>
   <si>
-    <t xml:space="preserve">Qty</t>
+    <t xml:space="preserve">Quantity</t>
   </si>
   <si>
     <t xml:space="preserve">Nikon D300</t>
@@ -162,7 +162,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>